<commit_message>
Minimal additions to subsystems
</commit_message>
<xml_diff>
--- a/Matt_Work/BiGG ID Additions/2015_06_11_rxns.xlsx
+++ b/Matt_Work/BiGG ID Additions/2015_06_11_rxns.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2452" uniqueCount="2047">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2460" uniqueCount="2049">
   <si>
     <t>rxn02483_c0</t>
   </si>
@@ -6158,6 +6158,12 @@
   </si>
   <si>
     <t>Glycogen Metabolism</t>
+  </si>
+  <si>
+    <t>Thioredoxin-disulfide Reductase; Pyrimidine Conversions</t>
+  </si>
+  <si>
+    <t>Sucrose Metabolism</t>
   </si>
 </sst>
 </file>
@@ -6214,14 +6220,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -6564,8 +6563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E667"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B651" sqref="B651"/>
+    <sheetView tabSelected="1" topLeftCell="A301" workbookViewId="0">
+      <selection activeCell="B313" sqref="B313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10822,6 +10821,9 @@
       <c r="A304" t="s">
         <v>865</v>
       </c>
+      <c r="B304" t="s">
+        <v>2047</v>
+      </c>
       <c r="D304" t="s">
         <v>867</v>
       </c>
@@ -10833,6 +10835,9 @@
       <c r="A305" t="s">
         <v>868</v>
       </c>
+      <c r="B305" s="1" t="s">
+        <v>1980</v>
+      </c>
       <c r="D305" t="s">
         <v>870</v>
       </c>
@@ -10844,6 +10849,9 @@
       <c r="A306" t="s">
         <v>871</v>
       </c>
+      <c r="B306" t="s">
+        <v>1982</v>
+      </c>
       <c r="D306" t="s">
         <v>873</v>
       </c>
@@ -10855,6 +10863,9 @@
       <c r="A307" t="s">
         <v>874</v>
       </c>
+      <c r="B307" t="s">
+        <v>1993</v>
+      </c>
       <c r="D307" t="s">
         <v>876</v>
       </c>
@@ -10866,6 +10877,9 @@
       <c r="A308" t="s">
         <v>877</v>
       </c>
+      <c r="B308" s="1" t="s">
+        <v>1974</v>
+      </c>
       <c r="D308" t="s">
         <v>878</v>
       </c>
@@ -10891,6 +10905,9 @@
       <c r="A310" t="s">
         <v>881</v>
       </c>
+      <c r="B310" t="s">
+        <v>2048</v>
+      </c>
       <c r="D310" t="s">
         <v>883</v>
       </c>
@@ -10902,6 +10919,9 @@
       <c r="A311" t="s">
         <v>884</v>
       </c>
+      <c r="B311" t="s">
+        <v>2031</v>
+      </c>
       <c r="D311" t="s">
         <v>885</v>
       </c>
@@ -10913,6 +10933,9 @@
       <c r="A312" t="s">
         <v>886</v>
       </c>
+      <c r="B312" t="s">
+        <v>1990</v>
+      </c>
       <c r="D312" t="s">
         <v>888</v>
       </c>
@@ -15268,7 +15291,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:B667">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>